<commit_message>
updated images and posts
</commit_message>
<xml_diff>
--- a/_data/research-projects.xlsx
+++ b/_data/research-projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93B6BF8-2CD9-43BA-B797-4F5BE10041A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF3CC45-3AA8-401D-AAD4-B6C4FDC5C0D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
   <si>
     <t>The objective of this project is to investigate the relationship between deformation of a foldable antenna and effective wavelength. Understanding this association could allow for remote sensing of curvature in flexible robots. Alternatively, the correlation between deformation and effective wavelength could be leveraged to create tunable foldable antennas using closed-loop control techniques.</t>
   </si>
@@ -268,7 +268,19 @@
     <t>efri</t>
   </si>
   <si>
-    <t>…</t>
+    <t>This  work  is  supported  by  Office  of  Naval  Research  Award  N00014-17-1-2117</t>
+  </si>
+  <si>
+    <t>SCRAM Platform 1</t>
+  </si>
+  <si>
+    <t>coming soon…</t>
+  </si>
+  <si>
+    <t>This work is supported by &lt;a href="https://www.nsf.gov/awardsearch/showAward?AWD_ID=1935324"&gt;NSF Award #1935324&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>This work is supported by &lt;a href="https://www.nsf.gov/awardsearch/showAward?AWD_ID=1841574"&gt;NSF Award #1841574&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -603,7 +615,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,6 +751,9 @@
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>71</v>
       </c>
@@ -756,6 +771,9 @@
       <c r="D9" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="H9" s="1" t="s">
         <v>72</v>
       </c>
@@ -927,13 +945,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
updated images and equipment
</commit_message>
<xml_diff>
--- a/_data/research-projects.xlsx
+++ b/_data/research-projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu.github.io\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DBF109-73E5-4956-AE84-7FF4BC9E92DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC29A8B4-9D1D-42BB-923B-4AAF59C3FD93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="24624" windowHeight="15768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="24624" windowHeight="15768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
   <si>
     <t>The objective of this project is to investigate the relationship between deformation of a foldable antenna and effective wavelength. Understanding this association could allow for remote sensing of curvature in flexible robots. Alternatively, the correlation between deformation and effective wavelength could be leveraged to create tunable foldable antennas using closed-loop control techniques.</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Funding for this project was provided in part by SRP.</t>
+  </si>
+  <si>
+    <t>/assets/images/research/cutter.png</t>
   </si>
 </sst>
 </file>
@@ -667,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -908,6 +911,9 @@
       <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
updated taha description, cole stuff
</commit_message>
<xml_diff>
--- a/_data/research-projects.xlsx
+++ b/_data/research-projects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu.github.io\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263EA813-A8E6-4B64-B441-13BF422493CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21D9B5-DBBD-4962-A529-629D2BB0C697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="33048" windowHeight="21648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
   <si>
     <t>The objective of this project is to investigate the relationship between deformation of a foldable antenna and effective wavelength. Understanding this association could allow for remote sensing of curvature in flexible robots. Alternatively, the correlation between deformation and effective wavelength could be leveraged to create tunable foldable antennas using closed-loop control techniques.</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Cole Brauer</t>
   </si>
   <si>
-    <t>This project is researching methods of automating the planning of multi-material manufacturing processes.  This research will be used to inform the development of a software planning tool that would aid in the development of low-cost educational robots.  The focus of this project is on processes that are widely available in educational institutions such as 3D printing and laser cutting.</t>
-  </si>
-  <si>
     <t>Force control offers numerous benefits to robots over other control schemes such as more natural movements and increased sensitivity to the surrounding environment, but it is typically only available to high-end robots. This research aims to develop a modular force control solution for low-cost robots. The solution is designed to be easy to incorporate into future laminate robots, allowing the designer to add force control capabilities, while placing minimal constraints on the design.</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
   </si>
   <si>
     <t>biped</t>
-  </si>
-  <si>
-    <t>misc</t>
   </si>
   <si>
     <t>onr</t>
@@ -324,6 +318,13 @@
   </si>
   <si>
     <t>Signals in the Soil</t>
+  </si>
+  <si>
+    <t>This project seeks to provide methods and set of tools for processing, modifying, and generating 3D models that use multiple materials and fabrication processes. Areas of research include planning of fabrication steps, automatic part modification, optimization of component properties, and generation of the files and fixtures needed to produce multi-material parts. Implementation of these algorithms is done in Python using a voxel-based model representation. This work will make multi-material fabrication more accessible for educational and research robotics.  Current work is focused on applications of graded materials in the design of robust material transitions. The results will inform the design of stronger flexible joints for use in low-cost robotics applications.  More information is available on the project GitHub repository. (https://github.com/cdbrauer/VoxelFuse)</t>
+  </si>
+  <si>
+    <t>Currently, a lot of focus previously for laminate robots has been on design, but more complex applications require higher level design. The aim of my project is to demonstrate that laminate robots can be utilized for higher level design by designing a laminate biped with model-based controls that can balance while standing and walking. This project starts from the early
+prototyping design stage. Designs are created using python and Solidworks; PopupCAD is used to produce the DXF files needed for high speed laminate manufacturing. Through testing various design iterations, a design was reached with the ability to stand. The motors of this design were then modified to meet desired torque parameters. Testing has shown high torque is necessary to utilize robust control techniques, which will be used to balance the biped while it both stands and walks. Through python-based physics simulations utilizing Kane’s method, a model of the bipedal design can be created and linearized for controls applications. Since the system is fully controllable, LQR control techniques will be applied for balancing while standing and walking.  Eventually, different control systems can be design and implemented for various system applications.</t>
   </si>
 </sst>
 </file>
@@ -673,49 +674,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="36.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="110.4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="102" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -724,12 +725,12 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="82.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -738,27 +739,27 @@
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="82.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="96.6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -769,56 +770,56 @@
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="55.2" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="55.2" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -829,19 +830,19 @@
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="82.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -852,44 +853,44 @@
         <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="69" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="55.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -898,36 +899,33 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="82.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="110.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -938,55 +936,46 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="82.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="69" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="102" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="124.2" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -995,35 +984,35 @@
         <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="151.80000000000001" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="96.6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
@@ -1032,41 +1021,41 @@
         <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="138" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="110.4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="102" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -1075,24 +1064,27 @@
         <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="153" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addding column for research project publications
</commit_message>
<xml_diff>
--- a/_data/research-projects.xlsx
+++ b/_data/research-projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu.github.io\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FF6A90-479D-43DC-A616-4A64728264D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435EB19B-C261-416E-9CD1-6DA18FB170D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15090" yWindow="12465" windowWidth="21600" windowHeight="11370" tabRatio="318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="research-projects" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="113">
   <si>
     <t>The objective of this project is to investigate the relationship between deformation of a foldable antenna and effective wavelength. Understanding this association could allow for remote sensing of curvature in flexible robots. Alternatively, the correlation between deformation and effective wavelength could be leveraged to create tunable foldable antennas using closed-loop control techniques.</t>
   </si>
@@ -377,6 +377,9 @@
   <si>
     <t>&lt;p&gt;This Faculty Early Career Development (CAREER) grant will make it possible to develop cost-effective, specialist robots that can be prototyped by a non-expert in a matter of hours. The goal of this project is to make robots more ubiquitous, accessible, and tunable for newcomers to robotics and for applications in industry, education, and academic research. Achieving this goal requires a shift towards more affordable materials, accessible fabrication strategies, and assistive design software that considers the particular dynamics of cost-efficient motors and materials, as well as the needs of specific applications. The results of this project will impact fields in which specialization is desirable, such as assistive robotics for the elderly, custom agricultural applications, and trash pickup in smart cities. The robots developed through this project will also serve as an affordable starting point for children to compete in after-school robotics competitions organized by local, youth-focused nonprofits. In addition, the models and templates developed for this project will be integrated into college-level robotics curricula, permitting students to venture deeper into advanced robotics topics earlier in their studies.&lt;/p&gt;
 &lt;p&gt;The fundamental research contribution of this project lies within the consideration and integration of compliant material systems into a unified design framework that supports the specialization and optimization of dynamical robotic systems. The research plan involves developing reduced models for the nonlinear mechanics of material systems that permit more affordable robot designs, and considering that compliance in simulations to customize, model, and optimize their performance. This approach will investigate machine learning techniques to automatically tune parametric, template-driven designs in a way that balances competing performance trade-offs like speed, payload, and efficiency. The project's research objectives include the representation of compliance, the utilization and understanding of compliance, the optimization of compliant systems, and validation of the framework through prototyping, experimental validation, and exemplar use-cases. The generality of the approach will be demonstrated by modeling and optimizing several subsystems of a bipedal robot.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>paper_keys</t>
   </si>
 </sst>
 </file>
@@ -724,23 +727,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -768,8 +772,11 @@
       <c r="I1" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="91" x14ac:dyDescent="0.35">
+      <c r="J1" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -789,7 +796,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -809,7 +816,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
@@ -829,7 +836,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -849,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>83</v>
       </c>
@@ -869,7 +876,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
@@ -892,7 +899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -915,7 +922,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -938,7 +945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="52" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -961,7 +968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="52" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -978,7 +985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1001,7 +1008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="104" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>90</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="104" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1070,7 +1077,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="117" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1093,7 +1100,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="143" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="91" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -1136,7 +1143,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="130" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1159,7 +1166,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="91" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="130" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
@@ -1199,7 +1206,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="104" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>98</v>
       </c>
@@ -1222,7 +1229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="247" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>102</v>
       </c>
@@ -1242,7 +1249,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="130" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>105</v>
       </c>

</xml_diff>